<commit_message>
Refatoração do código para permiter pesquisas com mais de 5 alternativas e permitir a escolha do delimitador da planilha
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\RPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\RPA_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51634924-F206-46AC-AC2E-FE3B5E9B3ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0676C5-B6F0-493F-881C-DC2553082CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Você prefere chocolate ao leite ou amargo?</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Options</t>
   </si>
   <si>
-    <t>Chocolate ao Leite, Chocolate Amargo</t>
-  </si>
-  <si>
     <t>Anônimo</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Tech</t>
   </si>
   <si>
-    <t>Humanas, Exatas</t>
-  </si>
-  <si>
     <t>Doces favoritos</t>
   </si>
   <si>
@@ -87,10 +81,28 @@
     <t>Sweet</t>
   </si>
   <si>
-    <t>Bolo, Sorverte, Chocolate, Pé de moleque</t>
-  </si>
-  <si>
     <t>Não</t>
+  </si>
+  <si>
+    <t>Qual seu número favorito</t>
+  </si>
+  <si>
+    <t>números !!!!!</t>
+  </si>
+  <si>
+    <t>Professor de matemática</t>
+  </si>
+  <si>
+    <t>Chocolate ao Leite; Chocolate Amargo</t>
+  </si>
+  <si>
+    <t>Humanas; Exatas</t>
+  </si>
+  <si>
+    <t>Bolo, Sorverte; Chocolate; Pé de moleque</t>
+  </si>
+  <si>
+    <t>1; 2; 3; 4; 5; 6; 7; 8; 9; 10; 11; 12; 13; 14; 15; 16</t>
   </si>
 </sst>
 </file>
@@ -156,8 +168,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC848D10-6023-4DFB-899A-1E4B2DD6A3A1}" name="Tabela2" displayName="Tabela2" ref="A1:H4" totalsRowShown="0">
-  <autoFilter ref="A1:H4" xr:uid="{DC848D10-6023-4DFB-899A-1E4B2DD6A3A1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DC848D10-6023-4DFB-899A-1E4B2DD6A3A1}" name="Tabela2" displayName="Tabela2" ref="A1:H5" totalsRowShown="0">
+  <autoFilter ref="A1:H5" xr:uid="{DC848D10-6023-4DFB-899A-1E4B2DD6A3A1}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FC138F1D-A015-455D-8F93-C8F4C07F6BC6}" name="título"/>
     <tableColumn id="2" xr3:uid="{2786A62E-C922-46F6-A151-58E1FECD7E0C}" name="Descrição" dataDxfId="1"/>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,16 +479,16 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -490,71 +502,97 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>